<commit_message>
add printing pf activity
</commit_message>
<xml_diff>
--- a/app/database/seeds/seed_files/masterfile.xlsx
+++ b/app/database/seeds/seed_files/masterfile.xlsx
@@ -56847,7 +56847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -58265,7 +58265,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60020,7 +60020,7 @@
   <dimension ref="A1:H153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>